<commit_message>
Update Tham chiếu, FRA,...
</commit_message>
<xml_diff>
--- a/Tham chiếu mã số.xlsx
+++ b/Tham chiếu mã số.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
   <si>
     <t>Mã</t>
   </si>
@@ -304,6 +304,282 @@
   </si>
   <si>
     <t>UCCN-1</t>
+  </si>
+  <si>
+    <t>Use case Tra cứu lịch phân công nhân viên</t>
+  </si>
+  <si>
+    <t>UCCN-2</t>
+  </si>
+  <si>
+    <t>UCCN-3</t>
+  </si>
+  <si>
+    <t>UCCN-4</t>
+  </si>
+  <si>
+    <t>UCCN-5</t>
+  </si>
+  <si>
+    <t>UCCN-6</t>
+  </si>
+  <si>
+    <t>UCCN-7</t>
+  </si>
+  <si>
+    <t>UCCN-8</t>
+  </si>
+  <si>
+    <t>UCCN-9</t>
+  </si>
+  <si>
+    <t>UCCN-10</t>
+  </si>
+  <si>
+    <t>UCCN-11</t>
+  </si>
+  <si>
+    <t>UCCN-12</t>
+  </si>
+  <si>
+    <t>UCCN-13</t>
+  </si>
+  <si>
+    <t>UCCN-14</t>
+  </si>
+  <si>
+    <t>UCCN-15</t>
+  </si>
+  <si>
+    <t>UCCN-16</t>
+  </si>
+  <si>
+    <t>UCCN-17</t>
+  </si>
+  <si>
+    <t>UCCN-18</t>
+  </si>
+  <si>
+    <t>UCCN-19</t>
+  </si>
+  <si>
+    <t>UCCN-20</t>
+  </si>
+  <si>
+    <t>UCCN-21</t>
+  </si>
+  <si>
+    <t>UCCN-22</t>
+  </si>
+  <si>
+    <t>UCCN-23</t>
+  </si>
+  <si>
+    <t>UCCN-24</t>
+  </si>
+  <si>
+    <t>UCCN-25</t>
+  </si>
+  <si>
+    <t>UCCN-26</t>
+  </si>
+  <si>
+    <t>UCCN-27</t>
+  </si>
+  <si>
+    <t>UCCN-28</t>
+  </si>
+  <si>
+    <t>UCCN-29</t>
+  </si>
+  <si>
+    <t>UCCN-30</t>
+  </si>
+  <si>
+    <t>UCCN-31</t>
+  </si>
+  <si>
+    <t>UCCN-32</t>
+  </si>
+  <si>
+    <t>UCCN-33</t>
+  </si>
+  <si>
+    <t>UCCN-34</t>
+  </si>
+  <si>
+    <t>UCCN-35</t>
+  </si>
+  <si>
+    <t>UCCN-36</t>
+  </si>
+  <si>
+    <t>UCCN-37</t>
+  </si>
+  <si>
+    <t>UCCN-38</t>
+  </si>
+  <si>
+    <t>UCCN-39</t>
+  </si>
+  <si>
+    <t>UCCN-40</t>
+  </si>
+  <si>
+    <t>UCCN-41</t>
+  </si>
+  <si>
+    <t>UCCN-42</t>
+  </si>
+  <si>
+    <t>UCCN-43</t>
+  </si>
+  <si>
+    <t>UCCN-44</t>
+  </si>
+  <si>
+    <t>UCCN-45</t>
+  </si>
+  <si>
+    <t>UCCN-46</t>
+  </si>
+  <si>
+    <t>Use case Lên lịch phân công nhân viên</t>
+  </si>
+  <si>
+    <t>Use case Cập nhật lịch phân công nhân viên</t>
+  </si>
+  <si>
+    <t>Use case Quản lí nhân viên (Thêm mới)</t>
+  </si>
+  <si>
+    <t>Use case Quản lí nhân viên (Xem)</t>
+  </si>
+  <si>
+    <t>Use case Quản lí nhân viên (Xóa)</t>
+  </si>
+  <si>
+    <t>Use case Quản lí nhân viên (Cập nhật)</t>
+  </si>
+  <si>
+    <t>Use case Quản lý dịch vụ</t>
+  </si>
+  <si>
+    <t>Use case Nhập thông tin đặt phòng offline</t>
+  </si>
+  <si>
+    <t>Use case Nhập thông tin đặt phòng online</t>
+  </si>
+  <si>
+    <t>Use case Chọn phòng cho khách hàng theo tiêu chí</t>
+  </si>
+  <si>
+    <t>Use case Đăng nhập</t>
+  </si>
+  <si>
+    <t>Use case Đăng xuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use case Đặt phòng offline </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use case Đặt phòng online </t>
+  </si>
+  <si>
+    <t>Use case Chat online</t>
+  </si>
+  <si>
+    <t>Use case Thanh toán offline</t>
+  </si>
+  <si>
+    <t>Use case Thanh toán online</t>
+  </si>
+  <si>
+    <t>Use case Nhắc nhở liên lạc khách hàng trước 5 ngày</t>
+  </si>
+  <si>
+    <t>Use case Nhắc nhở liên lạc khách hàng trước 2 ngày</t>
+  </si>
+  <si>
+    <t>Use case Hủy phòng offline</t>
+  </si>
+  <si>
+    <t>Use case Hủy phòng online</t>
+  </si>
+  <si>
+    <t>Use case Lập danh sách nhập hàng</t>
+  </si>
+  <si>
+    <t>Use case Thống kê thiết bị</t>
+  </si>
+  <si>
+    <t>Use case Quản lý thiết bị (Thêm mới)</t>
+  </si>
+  <si>
+    <t>Use case Quản lý thiết bị (Xóa)</t>
+  </si>
+  <si>
+    <t>Use case Quản lý thiết bị (Cập nhật)</t>
+  </si>
+  <si>
+    <t>Use case Quản lý thiết bị (Tra cứu)</t>
+  </si>
+  <si>
+    <t>Use case Đánh giá</t>
+  </si>
+  <si>
+    <t>Use case Tìm kiếm và tổng hợp thông tin theo ngày</t>
+  </si>
+  <si>
+    <t>Use case Tìm kiếm và tổng hợp thông tin theo tháng</t>
+  </si>
+  <si>
+    <t>Use case Tìm kiếm và tổng hợp thông tin theo quý</t>
+  </si>
+  <si>
+    <t>Use case Tìm kiếm và tổng hợp thông tin theo năm</t>
+  </si>
+  <si>
+    <t>Use case Tổng hợp</t>
+  </si>
+  <si>
+    <t>Use case So sánh dữ liệu</t>
+  </si>
+  <si>
+    <t>Use case Đăng kí tài khoản</t>
+  </si>
+  <si>
+    <t>Use case Đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Use case Đặt lại mật khẩu</t>
+  </si>
+  <si>
+    <t>Use case Xem lịch sử đặt phòng khách sạn</t>
+  </si>
+  <si>
+    <t>Use case Xem thông tin khách hàng</t>
+  </si>
+  <si>
+    <t>Use case Xem thông tin khách hàng (Nhân viên)</t>
+  </si>
+  <si>
+    <t>Use case Thêm khách hàng</t>
+  </si>
+  <si>
+    <t>Use case Cập nhật thông tin khách hàng</t>
+  </si>
+  <si>
+    <t>Use case Cập nhật thông tin khách hàng (Nhân viên)</t>
+  </si>
+  <si>
+    <t>Use case Xóa khách hàng</t>
+  </si>
+  <si>
+    <t>CLASS-1</t>
+  </si>
+  <si>
+    <t>Mô tả sơ đồ lớp ThongTinDatPhong</t>
   </si>
 </sst>
 </file>
@@ -365,15 +641,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -656,11 +935,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -671,10 +950,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33" x14ac:dyDescent="0.6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -789,267 +1068,638 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>